<commit_message>
Deploying to gh-pages from  @ 492b09b9039b1df2b57c4e36832567734b93215b 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/8.1.1.xlsx
+++ b/en/downloads/data-excel/8.1.1.xlsx
@@ -611,9 +611,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -622,7 +624,7 @@
     <col min="14" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="27" customHeight="1">
+    <row r="1" spans="1:14" ht="27" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -641,7 +643,7 @@
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:14">
       <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
@@ -660,7 +662,7 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="3"/>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
@@ -673,7 +675,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -713,8 +715,11 @@
       <c r="M4" s="14">
         <v>2019</v>
       </c>
+      <c r="N4" s="14">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" ht="31.5" customHeight="1" thickBot="1">
+    <row r="5" spans="1:14" ht="31.5" customHeight="1" thickBot="1">
       <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
@@ -754,8 +759,11 @@
       <c r="M5" s="17">
         <v>2.2999999999999998</v>
       </c>
+      <c r="N5" s="17">
+        <v>-10.199999999999999</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" customFormat="1">
+    <row r="6" spans="1:14" customFormat="1">
       <c r="A6" s="18"/>
       <c r="B6" s="19"/>
       <c r="C6" s="20"/>
@@ -770,12 +778,12 @@
       <c r="L6" s="21"/>
       <c r="M6" s="21"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:14">
       <c r="I10" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:14">
       <c r="I13" s="4" t="s">
         <v>12</v>
       </c>

</xml_diff>